<commit_message>
No requirement for NO_SEC flag for ESC14c Schannel 0x01 mapping
</commit_message>
<xml_diff>
--- a/ESC14-Table.xlsx
+++ b/ESC14-Table.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="687" documentId="8_{2482986A-DA8C-47E5-AF98-AD3D209F5F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4D3877-B5E2-4B16-80C6-995402B0F3B1}"/>
+  <xr:revisionPtr revIDLastSave="700" documentId="8_{2482986A-DA8C-47E5-AF98-AD3D209F5F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCB22236-83F8-40C0-9E65-D453EE2E5861}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{1C4A1DE5-D476-4BE3-BF39-CB4E97C10667}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="40">
   <si>
     <t>mail</t>
   </si>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8D3653-C941-454A-A67E-DF8E4FD8754B}">
   <dimension ref="A1:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection sqref="A1:U110"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5604,8 +5604,8 @@
       <c r="G75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H75" s="1" t="b">
-        <v>1</v>
+      <c r="H75" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>27</v>
@@ -5669,8 +5669,8 @@
       <c r="G76" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H76" s="1" t="b">
-        <v>1</v>
+      <c r="H76" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>27</v>
@@ -5734,8 +5734,8 @@
       <c r="G77" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H77" s="1" t="b">
-        <v>1</v>
+      <c r="H77" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>27</v>
@@ -5799,8 +5799,8 @@
       <c r="G78" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H78" s="1" t="b">
-        <v>1</v>
+      <c r="H78" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I78" s="1">
         <v>1</v>
@@ -5864,8 +5864,8 @@
       <c r="G79" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H79" s="1" t="b">
-        <v>1</v>
+      <c r="H79" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>27</v>
@@ -5929,8 +5929,8 @@
       <c r="G80" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H80" s="1" t="b">
-        <v>1</v>
+      <c r="H80" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>27</v>
@@ -5994,8 +5994,8 @@
       <c r="G81" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H81" s="1" t="b">
-        <v>1</v>
+      <c r="H81" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>27</v>
@@ -6059,8 +6059,8 @@
       <c r="G82" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H82" s="1" t="b">
-        <v>1</v>
+      <c r="H82" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I82" s="1">
         <v>1</v>
@@ -6124,8 +6124,8 @@
       <c r="G83" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H83" s="1" t="b">
-        <v>1</v>
+      <c r="H83" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>27</v>
@@ -6189,8 +6189,8 @@
       <c r="G84" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H84" s="1" t="b">
-        <v>1</v>
+      <c r="H84" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>27</v>
@@ -6254,8 +6254,8 @@
       <c r="G85" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H85" s="1" t="b">
-        <v>1</v>
+      <c r="H85" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>27</v>
@@ -6319,8 +6319,8 @@
       <c r="G86" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H86" s="1" t="b">
-        <v>1</v>
+      <c r="H86" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>

</xml_diff>